<commit_message>
Updated 05 to have parameters as well
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -296,11 +296,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +616,7 @@
     <col min="9" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
+    <row r="1" ht="14.95" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -638,7 +638,7 @@
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -658,7 +658,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -863,12 +863,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -967,7 +967,7 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
+    <row r="1" ht="14.95" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -991,7 +991,7 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>